<commit_message>
Use 3V3 reg with enable pin
</commit_message>
<xml_diff>
--- a/BMS Slave Files/BatMeas5.3 Manufacturing Files/Assembly/jlcpcb-bom.xlsx
+++ b/BMS Slave Files/BatMeas5.3 Manufacturing Files/Assembly/jlcpcb-bom.xlsx
@@ -217,7 +217,7 @@
     <t xml:space="preserve">3V3</t>
   </si>
   <si>
-    <t xml:space="preserve">C89347</t>
+    <t xml:space="preserve">C105222</t>
   </si>
   <si>
     <t xml:space="preserve">R10</t>
@@ -392,10 +392,10 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.55"/>

</xml_diff>